<commit_message>
Commented for the updated report
</commit_message>
<xml_diff>
--- a/target/classes/testdata/testdata.xlsx
+++ b/target/classes/testdata/testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="105">
   <si>
     <t>operation</t>
   </si>
@@ -303,9 +303,6 @@
     <t>//a[@id = 'ui-id-152']</t>
   </si>
   <si>
-    <t>//a[@id = 'ui-id-153']</t>
-  </si>
-  <si>
     <t>//a[@id = 'ui-id-156']</t>
   </si>
   <si>
@@ -328,12 +325,6 @@
   </si>
   <si>
     <t>Skate</t>
-  </si>
-  <si>
-    <t>https://vanssgstg.ada-asia.my/end-of-season-sales-jul24-sg.html</t>
-  </si>
-  <si>
-    <t>EOD sale</t>
   </si>
   <si>
     <t>mens</t>
@@ -1259,10 +1250,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56:C56"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,7 +1781,7 @@
         <v>87</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1832,7 +1823,7 @@
         <v>87</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1846,7 +1837,7 @@
         <v>87</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1888,7 +1879,7 @@
         <v>87</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1902,7 +1893,7 @@
         <v>87</v>
       </c>
       <c r="D47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1944,7 +1935,7 @@
         <v>87</v>
       </c>
       <c r="D50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1958,7 +1949,7 @@
         <v>87</v>
       </c>
       <c r="D51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2014,7 +2005,7 @@
         <v>87</v>
       </c>
       <c r="D55" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2028,62 +2019,6 @@
         <v>95</v>
       </c>
       <c r="D56" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C57" t="s">
-        <v>87</v>
-      </c>
-      <c r="D57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C58" t="s">
-        <v>87</v>
-      </c>
-      <c r="D58" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C59" t="s">
-        <v>87</v>
-      </c>
-      <c r="D59" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C60" t="s">
-        <v>96</v>
-      </c>
-      <c r="D60" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2104,7 +2039,7 @@
           <x14:formula1>
             <xm:f>temp!$F$2:$F$15</xm:f>
           </x14:formula1>
-          <xm:sqref>B2 B4:B26 B28:B60</xm:sqref>
+          <xm:sqref>B2 B4:B26 B28:B56</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>